<commit_message>
Printing methods ready, project code is ready
</commit_message>
<xml_diff>
--- a/Análisis/Patron para las coordenadas.xlsx
+++ b/Análisis/Patron para las coordenadas.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Desktop\2021\Segundo ciclo\Micro\Proyecto1Micro\Análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737892D4-0073-4C0F-8BDE-692370F5CE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002CCB17-2FB6-454E-9887-460F997AAD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7C3A939F-4E47-4EE8-A0B8-259C8FD34294}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7C3A939F-4E47-4EE8-A0B8-259C8FD34294}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Patron para las coordenadas" sheetId="1" r:id="rId1"/>
+    <sheet name="Imprimir coordenadas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,20 +35,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>←</t>
   </si>
+  <si>
+    <t>Coordenada plano normal</t>
+  </si>
+  <si>
+    <t>Coordenada matriz</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -227,11 +248,237 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,6 +654,70 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +726,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FF99FFCC"/>
+      <color rgb="FFCC99FF"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FFFFFF99"/>
-      <color rgb="FFCC99FF"/>
-      <color rgb="FF99FFCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -731,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CF5B13-17E0-457F-A968-EA9317FD12DE}">
   <dimension ref="B3:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,4 +2532,2795 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA25C15-A967-4643-93B6-32AD4FC6F54C}">
+  <dimension ref="B2:T104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J20:J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="93"/>
+    </row>
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="70"/>
+      <c r="D4" s="87">
+        <v>1</v>
+      </c>
+      <c r="E4" s="87">
+        <v>2</v>
+      </c>
+      <c r="F4" s="87">
+        <v>3</v>
+      </c>
+      <c r="G4" s="87">
+        <v>4</v>
+      </c>
+      <c r="H4" s="87">
+        <v>5</v>
+      </c>
+      <c r="I4" s="87">
+        <v>6</v>
+      </c>
+      <c r="J4" s="87">
+        <v>7</v>
+      </c>
+      <c r="K4" s="87">
+        <v>8</v>
+      </c>
+      <c r="L4" s="87">
+        <v>9</v>
+      </c>
+      <c r="M4" s="88">
+        <v>10</v>
+      </c>
+      <c r="P4" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" s="60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="71">
+        <v>1</v>
+      </c>
+      <c r="D5" s="79">
+        <v>100</v>
+      </c>
+      <c r="E5" s="80">
+        <v>99</v>
+      </c>
+      <c r="F5" s="76">
+        <v>98</v>
+      </c>
+      <c r="G5" s="84">
+        <v>97</v>
+      </c>
+      <c r="H5" s="79">
+        <v>96</v>
+      </c>
+      <c r="I5" s="80">
+        <v>95</v>
+      </c>
+      <c r="J5" s="76">
+        <v>94</v>
+      </c>
+      <c r="K5" s="84">
+        <v>93</v>
+      </c>
+      <c r="L5" s="79">
+        <v>92</v>
+      </c>
+      <c r="M5" s="89">
+        <v>91</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="66">
+        <v>0</v>
+      </c>
+      <c r="R5" s="61">
+        <v>6</v>
+      </c>
+      <c r="S5" s="62">
+        <v>5</v>
+      </c>
+      <c r="T5" s="23">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="94">
+        <v>2</v>
+      </c>
+      <c r="D6" s="68">
+        <v>65</v>
+      </c>
+      <c r="E6" s="79">
+        <v>64</v>
+      </c>
+      <c r="F6" s="80">
+        <v>63</v>
+      </c>
+      <c r="G6" s="76">
+        <v>62</v>
+      </c>
+      <c r="H6" s="84">
+        <v>61</v>
+      </c>
+      <c r="I6" s="79">
+        <v>60</v>
+      </c>
+      <c r="J6" s="80">
+        <v>59</v>
+      </c>
+      <c r="K6" s="76">
+        <v>58</v>
+      </c>
+      <c r="L6" s="85">
+        <v>57</v>
+      </c>
+      <c r="M6" s="74">
+        <v>90</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+      <c r="P6" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="66">
+        <v>0</v>
+      </c>
+      <c r="R6" s="61">
+        <v>6</v>
+      </c>
+      <c r="S6" s="62">
+        <v>6</v>
+      </c>
+      <c r="T6" s="23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="94">
+        <v>3</v>
+      </c>
+      <c r="D7" s="74">
+        <v>66</v>
+      </c>
+      <c r="E7" s="68">
+        <v>37</v>
+      </c>
+      <c r="F7" s="79">
+        <v>36</v>
+      </c>
+      <c r="G7" s="80">
+        <v>35</v>
+      </c>
+      <c r="H7" s="76">
+        <v>34</v>
+      </c>
+      <c r="I7" s="84">
+        <v>33</v>
+      </c>
+      <c r="J7" s="79">
+        <v>32</v>
+      </c>
+      <c r="K7" s="77">
+        <v>31</v>
+      </c>
+      <c r="L7" s="82">
+        <v>56</v>
+      </c>
+      <c r="M7" s="85">
+        <v>89</v>
+      </c>
+      <c r="O7" s="1">
+        <v>3</v>
+      </c>
+      <c r="P7" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="66">
+        <v>1</v>
+      </c>
+      <c r="R7" s="61">
+        <v>5</v>
+      </c>
+      <c r="S7" s="62">
+        <v>6</v>
+      </c>
+      <c r="T7" s="23">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="94">
+        <v>4</v>
+      </c>
+      <c r="D8" s="77">
+        <v>67</v>
+      </c>
+      <c r="E8" s="74">
+        <v>38</v>
+      </c>
+      <c r="F8" s="68">
+        <v>17</v>
+      </c>
+      <c r="G8" s="79">
+        <v>16</v>
+      </c>
+      <c r="H8" s="80">
+        <v>15</v>
+      </c>
+      <c r="I8" s="76">
+        <v>14</v>
+      </c>
+      <c r="J8" s="85">
+        <v>13</v>
+      </c>
+      <c r="K8" s="74">
+        <v>30</v>
+      </c>
+      <c r="L8" s="77">
+        <v>55</v>
+      </c>
+      <c r="M8" s="82">
+        <v>88</v>
+      </c>
+      <c r="O8" s="1">
+        <v>4</v>
+      </c>
+      <c r="P8" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="66">
+        <v>1</v>
+      </c>
+      <c r="R8" s="61">
+        <v>5</v>
+      </c>
+      <c r="S8" s="62">
+        <v>5</v>
+      </c>
+      <c r="T8" s="23">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="94">
+        <v>5</v>
+      </c>
+      <c r="D9" s="82">
+        <v>68</v>
+      </c>
+      <c r="E9" s="77">
+        <v>39</v>
+      </c>
+      <c r="F9" s="74">
+        <v>18</v>
+      </c>
+      <c r="G9" s="68">
+        <v>5</v>
+      </c>
+      <c r="H9" s="81">
+        <v>4</v>
+      </c>
+      <c r="I9" s="77">
+        <v>3</v>
+      </c>
+      <c r="J9" s="82">
+        <v>12</v>
+      </c>
+      <c r="K9" s="85">
+        <v>29</v>
+      </c>
+      <c r="L9" s="74">
+        <v>54</v>
+      </c>
+      <c r="M9" s="77">
+        <v>87</v>
+      </c>
+      <c r="O9" s="1">
+        <v>5</v>
+      </c>
+      <c r="P9" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q9" s="66">
+        <v>1</v>
+      </c>
+      <c r="R9" s="61">
+        <v>5</v>
+      </c>
+      <c r="S9" s="62">
+        <v>4</v>
+      </c>
+      <c r="T9" s="23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="73"/>
+      <c r="C10" s="94">
+        <v>6</v>
+      </c>
+      <c r="D10" s="85">
+        <v>69</v>
+      </c>
+      <c r="E10" s="82">
+        <v>40</v>
+      </c>
+      <c r="F10" s="77">
+        <v>19</v>
+      </c>
+      <c r="G10" s="74">
+        <v>6</v>
+      </c>
+      <c r="H10" s="75">
+        <v>1</v>
+      </c>
+      <c r="I10" s="78">
+        <v>2</v>
+      </c>
+      <c r="J10" s="77">
+        <v>11</v>
+      </c>
+      <c r="K10" s="82">
+        <v>28</v>
+      </c>
+      <c r="L10" s="85">
+        <v>53</v>
+      </c>
+      <c r="M10" s="74">
+        <v>86</v>
+      </c>
+      <c r="O10" s="1">
+        <v>6</v>
+      </c>
+      <c r="P10" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q10" s="66">
+        <v>0</v>
+      </c>
+      <c r="R10" s="61">
+        <v>6</v>
+      </c>
+      <c r="S10" s="62">
+        <v>4</v>
+      </c>
+      <c r="T10" s="23">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="94">
+        <v>7</v>
+      </c>
+      <c r="D11" s="74">
+        <v>70</v>
+      </c>
+      <c r="E11" s="85">
+        <v>41</v>
+      </c>
+      <c r="F11" s="82">
+        <v>20</v>
+      </c>
+      <c r="G11" s="83">
+        <v>7</v>
+      </c>
+      <c r="H11" s="79">
+        <v>8</v>
+      </c>
+      <c r="I11" s="84">
+        <v>9</v>
+      </c>
+      <c r="J11" s="78">
+        <v>10</v>
+      </c>
+      <c r="K11" s="77">
+        <v>27</v>
+      </c>
+      <c r="L11" s="82">
+        <v>52</v>
+      </c>
+      <c r="M11" s="85">
+        <v>85</v>
+      </c>
+      <c r="O11" s="1">
+        <v>7</v>
+      </c>
+      <c r="P11" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q11" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R11" s="61">
+        <v>7</v>
+      </c>
+      <c r="S11" s="62">
+        <v>4</v>
+      </c>
+      <c r="T11" s="23">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="94">
+        <v>8</v>
+      </c>
+      <c r="D12" s="77">
+        <v>71</v>
+      </c>
+      <c r="E12" s="74">
+        <v>42</v>
+      </c>
+      <c r="F12" s="86">
+        <v>21</v>
+      </c>
+      <c r="G12" s="76">
+        <v>22</v>
+      </c>
+      <c r="H12" s="80">
+        <v>23</v>
+      </c>
+      <c r="I12" s="79">
+        <v>24</v>
+      </c>
+      <c r="J12" s="84">
+        <v>25</v>
+      </c>
+      <c r="K12" s="78">
+        <v>26</v>
+      </c>
+      <c r="L12" s="77">
+        <v>51</v>
+      </c>
+      <c r="M12" s="82">
+        <v>84</v>
+      </c>
+      <c r="O12" s="1">
+        <v>8</v>
+      </c>
+      <c r="P12" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R12" s="61">
+        <v>7</v>
+      </c>
+      <c r="S12" s="62">
+        <v>5</v>
+      </c>
+      <c r="T12" s="23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="94">
+        <v>9</v>
+      </c>
+      <c r="D13" s="82">
+        <v>72</v>
+      </c>
+      <c r="E13" s="83">
+        <v>43</v>
+      </c>
+      <c r="F13" s="79">
+        <v>44</v>
+      </c>
+      <c r="G13" s="84">
+        <v>45</v>
+      </c>
+      <c r="H13" s="76">
+        <v>46</v>
+      </c>
+      <c r="I13" s="80">
+        <v>47</v>
+      </c>
+      <c r="J13" s="79">
+        <v>48</v>
+      </c>
+      <c r="K13" s="84">
+        <v>49</v>
+      </c>
+      <c r="L13" s="78">
+        <v>50</v>
+      </c>
+      <c r="M13" s="77">
+        <v>83</v>
+      </c>
+      <c r="O13" s="1">
+        <v>9</v>
+      </c>
+      <c r="P13" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R13" s="61">
+        <v>7</v>
+      </c>
+      <c r="S13" s="62">
+        <v>6</v>
+      </c>
+      <c r="T13" s="23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="72">
+        <v>10</v>
+      </c>
+      <c r="D14" s="86">
+        <v>73</v>
+      </c>
+      <c r="E14" s="76">
+        <v>74</v>
+      </c>
+      <c r="F14" s="80">
+        <v>75</v>
+      </c>
+      <c r="G14" s="79">
+        <v>76</v>
+      </c>
+      <c r="H14" s="84">
+        <v>77</v>
+      </c>
+      <c r="I14" s="76">
+        <v>78</v>
+      </c>
+      <c r="J14" s="80">
+        <v>79</v>
+      </c>
+      <c r="K14" s="79">
+        <v>80</v>
+      </c>
+      <c r="L14" s="84">
+        <v>81</v>
+      </c>
+      <c r="M14" s="78">
+        <v>82</v>
+      </c>
+      <c r="O14" s="1">
+        <v>10</v>
+      </c>
+      <c r="P14" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R14" s="61">
+        <v>7</v>
+      </c>
+      <c r="S14" s="62">
+        <v>7</v>
+      </c>
+      <c r="T14" s="23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="O15" s="1">
+        <v>11</v>
+      </c>
+      <c r="P15" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="66">
+        <v>0</v>
+      </c>
+      <c r="R15" s="61">
+        <v>6</v>
+      </c>
+      <c r="S15" s="62">
+        <v>7</v>
+      </c>
+      <c r="T15" s="23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="70"/>
+      <c r="D16" s="87">
+        <v>1</v>
+      </c>
+      <c r="E16" s="87">
+        <v>2</v>
+      </c>
+      <c r="F16" s="87">
+        <v>3</v>
+      </c>
+      <c r="G16" s="87">
+        <v>4</v>
+      </c>
+      <c r="H16" s="87">
+        <v>5</v>
+      </c>
+      <c r="I16" s="87">
+        <v>6</v>
+      </c>
+      <c r="J16" s="87">
+        <v>7</v>
+      </c>
+      <c r="K16" s="87">
+        <v>8</v>
+      </c>
+      <c r="L16" s="87">
+        <v>9</v>
+      </c>
+      <c r="M16" s="88">
+        <v>10</v>
+      </c>
+      <c r="O16" s="1">
+        <v>12</v>
+      </c>
+      <c r="P16" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="66">
+        <v>1</v>
+      </c>
+      <c r="R16" s="61">
+        <v>5</v>
+      </c>
+      <c r="S16" s="62">
+        <v>7</v>
+      </c>
+      <c r="T16" s="23">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="71">
+        <v>1</v>
+      </c>
+      <c r="D17" s="79">
+        <v>0</v>
+      </c>
+      <c r="E17" s="80">
+        <v>1</v>
+      </c>
+      <c r="F17" s="76">
+        <v>2</v>
+      </c>
+      <c r="G17" s="84">
+        <v>3</v>
+      </c>
+      <c r="H17" s="79">
+        <v>4</v>
+      </c>
+      <c r="I17" s="80">
+        <v>5</v>
+      </c>
+      <c r="J17" s="76">
+        <v>6</v>
+      </c>
+      <c r="K17" s="84">
+        <v>7</v>
+      </c>
+      <c r="L17" s="79">
+        <v>8</v>
+      </c>
+      <c r="M17" s="89">
+        <v>9</v>
+      </c>
+      <c r="O17" s="1">
+        <v>13</v>
+      </c>
+      <c r="P17" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>2</v>
+      </c>
+      <c r="R17" s="61">
+        <v>4</v>
+      </c>
+      <c r="S17" s="62">
+        <v>7</v>
+      </c>
+      <c r="T17" s="23">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="94">
+        <v>2</v>
+      </c>
+      <c r="D18" s="68">
+        <v>11</v>
+      </c>
+      <c r="E18" s="79">
+        <v>12</v>
+      </c>
+      <c r="F18" s="80">
+        <v>13</v>
+      </c>
+      <c r="G18" s="76">
+        <v>14</v>
+      </c>
+      <c r="H18" s="84">
+        <v>15</v>
+      </c>
+      <c r="I18" s="79">
+        <v>16</v>
+      </c>
+      <c r="J18" s="80">
+        <v>17</v>
+      </c>
+      <c r="K18" s="76">
+        <v>18</v>
+      </c>
+      <c r="L18" s="85">
+        <v>19</v>
+      </c>
+      <c r="M18" s="74">
+        <v>20</v>
+      </c>
+      <c r="O18" s="1">
+        <v>14</v>
+      </c>
+      <c r="P18" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="66">
+        <v>2</v>
+      </c>
+      <c r="R18" s="61">
+        <v>4</v>
+      </c>
+      <c r="S18" s="62">
+        <v>6</v>
+      </c>
+      <c r="T18" s="23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="94">
+        <v>3</v>
+      </c>
+      <c r="D19" s="74">
+        <v>22</v>
+      </c>
+      <c r="E19" s="68">
+        <v>23</v>
+      </c>
+      <c r="F19" s="79">
+        <v>24</v>
+      </c>
+      <c r="G19" s="80">
+        <v>25</v>
+      </c>
+      <c r="H19" s="76">
+        <v>26</v>
+      </c>
+      <c r="I19" s="84">
+        <v>27</v>
+      </c>
+      <c r="J19" s="79">
+        <v>28</v>
+      </c>
+      <c r="K19" s="77">
+        <v>29</v>
+      </c>
+      <c r="L19" s="82">
+        <v>30</v>
+      </c>
+      <c r="M19" s="85">
+        <v>31</v>
+      </c>
+      <c r="O19" s="1">
+        <v>15</v>
+      </c>
+      <c r="P19" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="66">
+        <v>2</v>
+      </c>
+      <c r="R19" s="61">
+        <v>4</v>
+      </c>
+      <c r="S19" s="62">
+        <v>5</v>
+      </c>
+      <c r="T19" s="23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="94">
+        <v>4</v>
+      </c>
+      <c r="D20" s="77">
+        <v>33</v>
+      </c>
+      <c r="E20" s="74">
+        <v>34</v>
+      </c>
+      <c r="F20" s="68">
+        <v>35</v>
+      </c>
+      <c r="G20" s="79">
+        <v>36</v>
+      </c>
+      <c r="H20" s="80">
+        <v>37</v>
+      </c>
+      <c r="I20" s="76">
+        <v>38</v>
+      </c>
+      <c r="J20" s="85">
+        <v>39</v>
+      </c>
+      <c r="K20" s="74">
+        <v>40</v>
+      </c>
+      <c r="L20" s="77">
+        <v>41</v>
+      </c>
+      <c r="M20" s="82">
+        <v>42</v>
+      </c>
+      <c r="O20" s="1">
+        <v>16</v>
+      </c>
+      <c r="P20" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q20" s="66">
+        <v>2</v>
+      </c>
+      <c r="R20" s="61">
+        <v>4</v>
+      </c>
+      <c r="S20" s="62">
+        <v>4</v>
+      </c>
+      <c r="T20" s="23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="94">
+        <v>5</v>
+      </c>
+      <c r="D21" s="82">
+        <v>44</v>
+      </c>
+      <c r="E21" s="77">
+        <v>45</v>
+      </c>
+      <c r="F21" s="74">
+        <v>46</v>
+      </c>
+      <c r="G21" s="68">
+        <v>47</v>
+      </c>
+      <c r="H21" s="81">
+        <v>48</v>
+      </c>
+      <c r="I21" s="77">
+        <v>49</v>
+      </c>
+      <c r="J21" s="82">
+        <v>50</v>
+      </c>
+      <c r="K21" s="85">
+        <v>51</v>
+      </c>
+      <c r="L21" s="74">
+        <v>52</v>
+      </c>
+      <c r="M21" s="77">
+        <v>53</v>
+      </c>
+      <c r="O21" s="1">
+        <v>17</v>
+      </c>
+      <c r="P21" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q21" s="66">
+        <v>2</v>
+      </c>
+      <c r="R21" s="61">
+        <v>4</v>
+      </c>
+      <c r="S21" s="62">
+        <v>3</v>
+      </c>
+      <c r="T21" s="23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="94">
+        <v>6</v>
+      </c>
+      <c r="D22" s="85">
+        <v>55</v>
+      </c>
+      <c r="E22" s="82">
+        <v>56</v>
+      </c>
+      <c r="F22" s="77">
+        <v>57</v>
+      </c>
+      <c r="G22" s="74">
+        <v>58</v>
+      </c>
+      <c r="H22" s="75">
+        <v>59</v>
+      </c>
+      <c r="I22" s="78">
+        <v>60</v>
+      </c>
+      <c r="J22" s="77">
+        <v>61</v>
+      </c>
+      <c r="K22" s="82">
+        <v>62</v>
+      </c>
+      <c r="L22" s="85">
+        <v>63</v>
+      </c>
+      <c r="M22" s="74">
+        <v>64</v>
+      </c>
+      <c r="O22" s="1">
+        <v>18</v>
+      </c>
+      <c r="P22" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q22" s="66">
+        <v>1</v>
+      </c>
+      <c r="R22" s="61">
+        <v>5</v>
+      </c>
+      <c r="S22" s="62">
+        <v>3</v>
+      </c>
+      <c r="T22" s="23">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="94">
+        <v>7</v>
+      </c>
+      <c r="D23" s="74">
+        <v>66</v>
+      </c>
+      <c r="E23" s="85">
+        <v>67</v>
+      </c>
+      <c r="F23" s="82">
+        <v>68</v>
+      </c>
+      <c r="G23" s="83">
+        <v>69</v>
+      </c>
+      <c r="H23" s="79">
+        <v>70</v>
+      </c>
+      <c r="I23" s="84">
+        <v>71</v>
+      </c>
+      <c r="J23" s="78">
+        <v>72</v>
+      </c>
+      <c r="K23" s="77">
+        <v>73</v>
+      </c>
+      <c r="L23" s="82">
+        <v>74</v>
+      </c>
+      <c r="M23" s="85">
+        <v>75</v>
+      </c>
+      <c r="O23" s="1">
+        <v>19</v>
+      </c>
+      <c r="P23" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q23" s="66">
+        <v>0</v>
+      </c>
+      <c r="R23" s="61">
+        <v>6</v>
+      </c>
+      <c r="S23" s="62">
+        <v>3</v>
+      </c>
+      <c r="T23" s="23">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="94">
+        <v>8</v>
+      </c>
+      <c r="D24" s="77">
+        <v>77</v>
+      </c>
+      <c r="E24" s="74">
+        <v>78</v>
+      </c>
+      <c r="F24" s="86">
+        <v>79</v>
+      </c>
+      <c r="G24" s="76">
+        <v>80</v>
+      </c>
+      <c r="H24" s="80">
+        <v>81</v>
+      </c>
+      <c r="I24" s="79">
+        <v>82</v>
+      </c>
+      <c r="J24" s="84">
+        <v>83</v>
+      </c>
+      <c r="K24" s="78">
+        <v>84</v>
+      </c>
+      <c r="L24" s="77">
+        <v>85</v>
+      </c>
+      <c r="M24" s="82">
+        <v>86</v>
+      </c>
+      <c r="O24" s="1">
+        <v>20</v>
+      </c>
+      <c r="P24" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q24" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R24" s="61">
+        <v>7</v>
+      </c>
+      <c r="S24" s="62">
+        <v>3</v>
+      </c>
+      <c r="T24" s="23">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="94">
+        <v>9</v>
+      </c>
+      <c r="D25" s="82">
+        <v>88</v>
+      </c>
+      <c r="E25" s="83">
+        <v>89</v>
+      </c>
+      <c r="F25" s="79">
+        <v>90</v>
+      </c>
+      <c r="G25" s="84">
+        <v>91</v>
+      </c>
+      <c r="H25" s="76">
+        <v>92</v>
+      </c>
+      <c r="I25" s="80">
+        <v>93</v>
+      </c>
+      <c r="J25" s="79">
+        <v>94</v>
+      </c>
+      <c r="K25" s="84">
+        <v>95</v>
+      </c>
+      <c r="L25" s="78">
+        <v>96</v>
+      </c>
+      <c r="M25" s="77">
+        <v>97</v>
+      </c>
+      <c r="O25" s="1">
+        <v>21</v>
+      </c>
+      <c r="P25" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q25" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R25" s="61">
+        <v>8</v>
+      </c>
+      <c r="S25" s="62">
+        <v>3</v>
+      </c>
+      <c r="T25" s="23">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="72">
+        <v>10</v>
+      </c>
+      <c r="D26" s="86">
+        <v>99</v>
+      </c>
+      <c r="E26" s="76">
+        <v>100</v>
+      </c>
+      <c r="F26" s="80">
+        <v>101</v>
+      </c>
+      <c r="G26" s="79">
+        <v>102</v>
+      </c>
+      <c r="H26" s="84">
+        <v>103</v>
+      </c>
+      <c r="I26" s="76">
+        <v>104</v>
+      </c>
+      <c r="J26" s="80">
+        <v>105</v>
+      </c>
+      <c r="K26" s="79">
+        <v>106</v>
+      </c>
+      <c r="L26" s="84">
+        <v>107</v>
+      </c>
+      <c r="M26" s="78">
+        <v>108</v>
+      </c>
+      <c r="O26" s="1">
+        <v>22</v>
+      </c>
+      <c r="P26" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q26" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R26" s="61">
+        <v>8</v>
+      </c>
+      <c r="S26" s="62">
+        <v>4</v>
+      </c>
+      <c r="T26" s="23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O27" s="1">
+        <v>23</v>
+      </c>
+      <c r="P27" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R27" s="61">
+        <v>8</v>
+      </c>
+      <c r="S27" s="62">
+        <v>5</v>
+      </c>
+      <c r="T27" s="23">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O28" s="1">
+        <v>24</v>
+      </c>
+      <c r="P28" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R28" s="61">
+        <v>8</v>
+      </c>
+      <c r="S28" s="62">
+        <v>6</v>
+      </c>
+      <c r="T28" s="23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O29" s="1">
+        <v>25</v>
+      </c>
+      <c r="P29" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R29" s="61">
+        <v>8</v>
+      </c>
+      <c r="S29" s="62">
+        <v>7</v>
+      </c>
+      <c r="T29" s="23">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O30" s="1">
+        <v>26</v>
+      </c>
+      <c r="P30" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R30" s="61">
+        <v>8</v>
+      </c>
+      <c r="S30" s="62">
+        <v>8</v>
+      </c>
+      <c r="T30" s="23">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O31" s="1">
+        <v>27</v>
+      </c>
+      <c r="P31" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R31" s="61">
+        <v>7</v>
+      </c>
+      <c r="S31" s="62">
+        <v>8</v>
+      </c>
+      <c r="T31" s="23">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O32" s="1">
+        <v>28</v>
+      </c>
+      <c r="P32" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="66">
+        <v>0</v>
+      </c>
+      <c r="R32" s="61">
+        <v>6</v>
+      </c>
+      <c r="S32" s="62">
+        <v>8</v>
+      </c>
+      <c r="T32" s="23">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O33" s="1">
+        <v>29</v>
+      </c>
+      <c r="P33" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="66">
+        <v>1</v>
+      </c>
+      <c r="R33" s="61">
+        <v>5</v>
+      </c>
+      <c r="S33" s="62">
+        <v>8</v>
+      </c>
+      <c r="T33" s="23">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O34" s="1">
+        <v>30</v>
+      </c>
+      <c r="P34" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="66">
+        <v>2</v>
+      </c>
+      <c r="R34" s="61">
+        <v>4</v>
+      </c>
+      <c r="S34" s="62">
+        <v>8</v>
+      </c>
+      <c r="T34" s="23">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O35" s="1">
+        <v>31</v>
+      </c>
+      <c r="P35" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q35" s="66">
+        <v>3</v>
+      </c>
+      <c r="R35" s="61">
+        <v>3</v>
+      </c>
+      <c r="S35" s="62">
+        <v>8</v>
+      </c>
+      <c r="T35" s="23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O36" s="1">
+        <v>32</v>
+      </c>
+      <c r="P36" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="66">
+        <v>3</v>
+      </c>
+      <c r="R36" s="61">
+        <v>3</v>
+      </c>
+      <c r="S36" s="62">
+        <v>7</v>
+      </c>
+      <c r="T36" s="23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O37" s="1">
+        <v>33</v>
+      </c>
+      <c r="P37" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="66">
+        <v>3</v>
+      </c>
+      <c r="R37" s="61">
+        <v>3</v>
+      </c>
+      <c r="S37" s="62">
+        <v>6</v>
+      </c>
+      <c r="T37" s="23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O38" s="1">
+        <v>34</v>
+      </c>
+      <c r="P38" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="66">
+        <v>3</v>
+      </c>
+      <c r="R38" s="61">
+        <v>3</v>
+      </c>
+      <c r="S38" s="62">
+        <v>5</v>
+      </c>
+      <c r="T38" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O39" s="1">
+        <v>35</v>
+      </c>
+      <c r="P39" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q39" s="66">
+        <v>3</v>
+      </c>
+      <c r="R39" s="61">
+        <v>3</v>
+      </c>
+      <c r="S39" s="62">
+        <v>4</v>
+      </c>
+      <c r="T39" s="23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O40" s="1">
+        <v>36</v>
+      </c>
+      <c r="P40" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q40" s="66">
+        <v>3</v>
+      </c>
+      <c r="R40" s="61">
+        <v>3</v>
+      </c>
+      <c r="S40" s="62">
+        <v>3</v>
+      </c>
+      <c r="T40" s="23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O41" s="1">
+        <v>37</v>
+      </c>
+      <c r="P41" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q41" s="66">
+        <v>3</v>
+      </c>
+      <c r="R41" s="61">
+        <v>3</v>
+      </c>
+      <c r="S41" s="62">
+        <v>2</v>
+      </c>
+      <c r="T41" s="23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O42" s="1">
+        <v>38</v>
+      </c>
+      <c r="P42" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q42" s="66">
+        <v>2</v>
+      </c>
+      <c r="R42" s="61">
+        <v>4</v>
+      </c>
+      <c r="S42" s="62">
+        <v>2</v>
+      </c>
+      <c r="T42" s="23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O43" s="1">
+        <v>39</v>
+      </c>
+      <c r="P43" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q43" s="66">
+        <v>1</v>
+      </c>
+      <c r="R43" s="61">
+        <v>5</v>
+      </c>
+      <c r="S43" s="62">
+        <v>2</v>
+      </c>
+      <c r="T43" s="23">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O44" s="1">
+        <v>40</v>
+      </c>
+      <c r="P44" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q44" s="66">
+        <v>0</v>
+      </c>
+      <c r="R44" s="61">
+        <v>6</v>
+      </c>
+      <c r="S44" s="62">
+        <v>2</v>
+      </c>
+      <c r="T44" s="23">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O45" s="1">
+        <v>41</v>
+      </c>
+      <c r="P45" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q45" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="61">
+        <v>7</v>
+      </c>
+      <c r="S45" s="62">
+        <v>2</v>
+      </c>
+      <c r="T45" s="23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O46" s="1">
+        <v>42</v>
+      </c>
+      <c r="P46" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q46" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R46" s="61">
+        <v>8</v>
+      </c>
+      <c r="S46" s="62">
+        <v>2</v>
+      </c>
+      <c r="T46" s="23">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O47" s="1">
+        <v>43</v>
+      </c>
+      <c r="P47" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q47" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R47" s="61">
+        <v>9</v>
+      </c>
+      <c r="S47" s="62">
+        <v>2</v>
+      </c>
+      <c r="T47" s="23">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O48" s="1">
+        <v>44</v>
+      </c>
+      <c r="P48" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q48" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R48" s="61">
+        <v>9</v>
+      </c>
+      <c r="S48" s="62">
+        <v>3</v>
+      </c>
+      <c r="T48" s="23">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O49" s="1">
+        <v>45</v>
+      </c>
+      <c r="P49" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q49" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R49" s="61">
+        <v>9</v>
+      </c>
+      <c r="S49" s="62">
+        <v>4</v>
+      </c>
+      <c r="T49" s="23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O50" s="1">
+        <v>46</v>
+      </c>
+      <c r="P50" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R50" s="61">
+        <v>9</v>
+      </c>
+      <c r="S50" s="62">
+        <v>5</v>
+      </c>
+      <c r="T50" s="23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O51" s="1">
+        <v>47</v>
+      </c>
+      <c r="P51" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R51" s="61">
+        <v>9</v>
+      </c>
+      <c r="S51" s="62">
+        <v>6</v>
+      </c>
+      <c r="T51" s="23">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O52" s="1">
+        <v>48</v>
+      </c>
+      <c r="P52" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q52" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R52" s="61">
+        <v>9</v>
+      </c>
+      <c r="S52" s="62">
+        <v>7</v>
+      </c>
+      <c r="T52" s="23">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O53" s="1">
+        <v>49</v>
+      </c>
+      <c r="P53" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q53" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R53" s="61">
+        <v>9</v>
+      </c>
+      <c r="S53" s="62">
+        <v>8</v>
+      </c>
+      <c r="T53" s="23">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O54" s="1">
+        <v>50</v>
+      </c>
+      <c r="P54" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q54" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R54" s="61">
+        <v>9</v>
+      </c>
+      <c r="S54" s="62">
+        <v>9</v>
+      </c>
+      <c r="T54" s="23">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O55" s="1">
+        <v>51</v>
+      </c>
+      <c r="P55" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q55" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R55" s="61">
+        <v>8</v>
+      </c>
+      <c r="S55" s="62">
+        <v>9</v>
+      </c>
+      <c r="T55" s="23">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O56" s="1">
+        <v>52</v>
+      </c>
+      <c r="P56" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q56" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R56" s="61">
+        <v>7</v>
+      </c>
+      <c r="S56" s="62">
+        <v>9</v>
+      </c>
+      <c r="T56" s="23">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O57" s="1">
+        <v>53</v>
+      </c>
+      <c r="P57" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="66">
+        <v>0</v>
+      </c>
+      <c r="R57" s="61">
+        <v>6</v>
+      </c>
+      <c r="S57" s="62">
+        <v>9</v>
+      </c>
+      <c r="T57" s="23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O58" s="1">
+        <v>54</v>
+      </c>
+      <c r="P58" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q58" s="66">
+        <v>1</v>
+      </c>
+      <c r="R58" s="61">
+        <v>5</v>
+      </c>
+      <c r="S58" s="62">
+        <v>9</v>
+      </c>
+      <c r="T58" s="23">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O59" s="1">
+        <v>55</v>
+      </c>
+      <c r="P59" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q59" s="66">
+        <v>2</v>
+      </c>
+      <c r="R59" s="61">
+        <v>4</v>
+      </c>
+      <c r="S59" s="62">
+        <v>9</v>
+      </c>
+      <c r="T59" s="23">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O60" s="1">
+        <v>56</v>
+      </c>
+      <c r="P60" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q60" s="66">
+        <v>3</v>
+      </c>
+      <c r="R60" s="61">
+        <v>3</v>
+      </c>
+      <c r="S60" s="62">
+        <v>9</v>
+      </c>
+      <c r="T60" s="23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O61" s="1">
+        <v>57</v>
+      </c>
+      <c r="P61" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q61" s="66">
+        <v>4</v>
+      </c>
+      <c r="R61" s="61">
+        <v>2</v>
+      </c>
+      <c r="S61" s="62">
+        <v>9</v>
+      </c>
+      <c r="T61" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O62" s="1">
+        <v>58</v>
+      </c>
+      <c r="P62" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q62" s="66">
+        <v>4</v>
+      </c>
+      <c r="R62" s="61">
+        <v>2</v>
+      </c>
+      <c r="S62" s="62">
+        <v>8</v>
+      </c>
+      <c r="T62" s="23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O63" s="1">
+        <v>59</v>
+      </c>
+      <c r="P63" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q63" s="66">
+        <v>4</v>
+      </c>
+      <c r="R63" s="61">
+        <v>2</v>
+      </c>
+      <c r="S63" s="62">
+        <v>7</v>
+      </c>
+      <c r="T63" s="23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O64" s="1">
+        <v>60</v>
+      </c>
+      <c r="P64" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="66">
+        <v>4</v>
+      </c>
+      <c r="R64" s="61">
+        <v>2</v>
+      </c>
+      <c r="S64" s="62">
+        <v>6</v>
+      </c>
+      <c r="T64" s="23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O65" s="1">
+        <v>61</v>
+      </c>
+      <c r="P65" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="66">
+        <v>4</v>
+      </c>
+      <c r="R65" s="61">
+        <v>2</v>
+      </c>
+      <c r="S65" s="62">
+        <v>5</v>
+      </c>
+      <c r="T65" s="23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O66" s="1">
+        <v>62</v>
+      </c>
+      <c r="P66" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q66" s="66">
+        <v>4</v>
+      </c>
+      <c r="R66" s="61">
+        <v>2</v>
+      </c>
+      <c r="S66" s="62">
+        <v>4</v>
+      </c>
+      <c r="T66" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O67" s="1">
+        <v>63</v>
+      </c>
+      <c r="P67" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q67" s="66">
+        <v>4</v>
+      </c>
+      <c r="R67" s="61">
+        <v>2</v>
+      </c>
+      <c r="S67" s="62">
+        <v>3</v>
+      </c>
+      <c r="T67" s="23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O68" s="1">
+        <v>64</v>
+      </c>
+      <c r="P68" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q68" s="66">
+        <v>4</v>
+      </c>
+      <c r="R68" s="61">
+        <v>2</v>
+      </c>
+      <c r="S68" s="62">
+        <v>2</v>
+      </c>
+      <c r="T68" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O69" s="1">
+        <v>65</v>
+      </c>
+      <c r="P69" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q69" s="66">
+        <v>4</v>
+      </c>
+      <c r="R69" s="61">
+        <v>2</v>
+      </c>
+      <c r="S69" s="62">
+        <v>1</v>
+      </c>
+      <c r="T69" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O70" s="1">
+        <v>66</v>
+      </c>
+      <c r="P70" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q70" s="66">
+        <v>3</v>
+      </c>
+      <c r="R70" s="61">
+        <v>3</v>
+      </c>
+      <c r="S70" s="62">
+        <v>1</v>
+      </c>
+      <c r="T70" s="23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O71" s="1">
+        <v>67</v>
+      </c>
+      <c r="P71" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q71" s="66">
+        <v>2</v>
+      </c>
+      <c r="R71" s="61">
+        <v>4</v>
+      </c>
+      <c r="S71" s="62">
+        <v>1</v>
+      </c>
+      <c r="T71" s="23">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O72" s="1">
+        <v>68</v>
+      </c>
+      <c r="P72" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q72" s="66">
+        <v>1</v>
+      </c>
+      <c r="R72" s="61">
+        <v>5</v>
+      </c>
+      <c r="S72" s="62">
+        <v>1</v>
+      </c>
+      <c r="T72" s="23">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O73" s="1">
+        <v>69</v>
+      </c>
+      <c r="P73" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q73" s="66">
+        <v>0</v>
+      </c>
+      <c r="R73" s="61">
+        <v>6</v>
+      </c>
+      <c r="S73" s="62">
+        <v>1</v>
+      </c>
+      <c r="T73" s="23">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O74" s="1">
+        <v>70</v>
+      </c>
+      <c r="P74" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q74" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="61">
+        <v>7</v>
+      </c>
+      <c r="S74" s="62">
+        <v>1</v>
+      </c>
+      <c r="T74" s="23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O75" s="1">
+        <v>71</v>
+      </c>
+      <c r="P75" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q75" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R75" s="61">
+        <v>8</v>
+      </c>
+      <c r="S75" s="62">
+        <v>1</v>
+      </c>
+      <c r="T75" s="23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O76" s="1">
+        <v>72</v>
+      </c>
+      <c r="P76" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q76" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R76" s="61">
+        <v>9</v>
+      </c>
+      <c r="S76" s="62">
+        <v>1</v>
+      </c>
+      <c r="T76" s="23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O77" s="1">
+        <v>73</v>
+      </c>
+      <c r="P77" s="61">
+        <v>-4</v>
+      </c>
+      <c r="Q77" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R77" s="61">
+        <v>10</v>
+      </c>
+      <c r="S77" s="62">
+        <v>1</v>
+      </c>
+      <c r="T77" s="23">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O78" s="1">
+        <v>74</v>
+      </c>
+      <c r="P78" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q78" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R78" s="61">
+        <v>10</v>
+      </c>
+      <c r="S78" s="62">
+        <v>2</v>
+      </c>
+      <c r="T78" s="23">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O79" s="1">
+        <v>75</v>
+      </c>
+      <c r="P79" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q79" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R79" s="61">
+        <v>10</v>
+      </c>
+      <c r="S79" s="62">
+        <v>3</v>
+      </c>
+      <c r="T79" s="23">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O80" s="1">
+        <v>76</v>
+      </c>
+      <c r="P80" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q80" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R80" s="61">
+        <v>10</v>
+      </c>
+      <c r="S80" s="62">
+        <v>4</v>
+      </c>
+      <c r="T80" s="23">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O81" s="1">
+        <v>77</v>
+      </c>
+      <c r="P81" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R81" s="61">
+        <v>10</v>
+      </c>
+      <c r="S81" s="62">
+        <v>5</v>
+      </c>
+      <c r="T81" s="23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O82" s="1">
+        <v>78</v>
+      </c>
+      <c r="P82" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R82" s="61">
+        <v>10</v>
+      </c>
+      <c r="S82" s="62">
+        <v>6</v>
+      </c>
+      <c r="T82" s="23">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O83" s="1">
+        <v>79</v>
+      </c>
+      <c r="P83" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q83" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R83" s="61">
+        <v>10</v>
+      </c>
+      <c r="S83" s="62">
+        <v>7</v>
+      </c>
+      <c r="T83" s="23">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O84" s="1">
+        <v>80</v>
+      </c>
+      <c r="P84" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q84" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R84" s="61">
+        <v>10</v>
+      </c>
+      <c r="S84" s="62">
+        <v>8</v>
+      </c>
+      <c r="T84" s="23">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O85" s="1">
+        <v>81</v>
+      </c>
+      <c r="P85" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q85" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R85" s="61">
+        <v>10</v>
+      </c>
+      <c r="S85" s="62">
+        <v>9</v>
+      </c>
+      <c r="T85" s="23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O86" s="1">
+        <v>82</v>
+      </c>
+      <c r="P86" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q86" s="66">
+        <v>-4</v>
+      </c>
+      <c r="R86" s="61">
+        <v>10</v>
+      </c>
+      <c r="S86" s="62">
+        <v>10</v>
+      </c>
+      <c r="T86" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O87" s="1">
+        <v>83</v>
+      </c>
+      <c r="P87" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q87" s="66">
+        <v>-3</v>
+      </c>
+      <c r="R87" s="61">
+        <v>9</v>
+      </c>
+      <c r="S87" s="62">
+        <v>10</v>
+      </c>
+      <c r="T87" s="23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O88" s="1">
+        <v>84</v>
+      </c>
+      <c r="P88" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q88" s="66">
+        <v>-2</v>
+      </c>
+      <c r="R88" s="61">
+        <v>8</v>
+      </c>
+      <c r="S88" s="62">
+        <v>10</v>
+      </c>
+      <c r="T88" s="23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O89" s="1">
+        <v>85</v>
+      </c>
+      <c r="P89" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q89" s="66">
+        <v>-1</v>
+      </c>
+      <c r="R89" s="61">
+        <v>7</v>
+      </c>
+      <c r="S89" s="62">
+        <v>10</v>
+      </c>
+      <c r="T89" s="23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O90" s="1">
+        <v>86</v>
+      </c>
+      <c r="P90" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q90" s="66">
+        <v>0</v>
+      </c>
+      <c r="R90" s="61">
+        <v>6</v>
+      </c>
+      <c r="S90" s="62">
+        <v>10</v>
+      </c>
+      <c r="T90" s="23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O91" s="1">
+        <v>87</v>
+      </c>
+      <c r="P91" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q91" s="66">
+        <v>1</v>
+      </c>
+      <c r="R91" s="61">
+        <v>5</v>
+      </c>
+      <c r="S91" s="62">
+        <v>10</v>
+      </c>
+      <c r="T91" s="23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O92" s="1">
+        <v>88</v>
+      </c>
+      <c r="P92" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q92" s="66">
+        <v>2</v>
+      </c>
+      <c r="R92" s="61">
+        <v>4</v>
+      </c>
+      <c r="S92" s="62">
+        <v>10</v>
+      </c>
+      <c r="T92" s="23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O93" s="1">
+        <v>89</v>
+      </c>
+      <c r="P93" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q93" s="66">
+        <v>3</v>
+      </c>
+      <c r="R93" s="61">
+        <v>3</v>
+      </c>
+      <c r="S93" s="62">
+        <v>10</v>
+      </c>
+      <c r="T93" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O94" s="1">
+        <v>90</v>
+      </c>
+      <c r="P94" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q94" s="66">
+        <v>4</v>
+      </c>
+      <c r="R94" s="61">
+        <v>2</v>
+      </c>
+      <c r="S94" s="62">
+        <v>10</v>
+      </c>
+      <c r="T94" s="23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O95" s="1">
+        <v>91</v>
+      </c>
+      <c r="P95" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q95" s="66">
+        <v>5</v>
+      </c>
+      <c r="R95" s="61">
+        <v>1</v>
+      </c>
+      <c r="S95" s="62">
+        <v>10</v>
+      </c>
+      <c r="T95" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O96" s="1">
+        <v>92</v>
+      </c>
+      <c r="P96" s="61">
+        <v>4</v>
+      </c>
+      <c r="Q96" s="66">
+        <v>5</v>
+      </c>
+      <c r="R96" s="61">
+        <v>1</v>
+      </c>
+      <c r="S96" s="62">
+        <v>9</v>
+      </c>
+      <c r="T96" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O97" s="1">
+        <v>93</v>
+      </c>
+      <c r="P97" s="61">
+        <v>3</v>
+      </c>
+      <c r="Q97" s="66">
+        <v>5</v>
+      </c>
+      <c r="R97" s="61">
+        <v>1</v>
+      </c>
+      <c r="S97" s="62">
+        <v>8</v>
+      </c>
+      <c r="T97" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O98" s="1">
+        <v>94</v>
+      </c>
+      <c r="P98" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q98" s="66">
+        <v>5</v>
+      </c>
+      <c r="R98" s="61">
+        <v>1</v>
+      </c>
+      <c r="S98" s="62">
+        <v>7</v>
+      </c>
+      <c r="T98" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O99" s="1">
+        <v>95</v>
+      </c>
+      <c r="P99" s="61">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="66">
+        <v>5</v>
+      </c>
+      <c r="R99" s="61">
+        <v>1</v>
+      </c>
+      <c r="S99" s="62">
+        <v>6</v>
+      </c>
+      <c r="T99" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O100" s="1">
+        <v>96</v>
+      </c>
+      <c r="P100" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="66">
+        <v>5</v>
+      </c>
+      <c r="R100" s="61">
+        <v>1</v>
+      </c>
+      <c r="S100" s="62">
+        <v>5</v>
+      </c>
+      <c r="T100" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O101" s="1">
+        <v>97</v>
+      </c>
+      <c r="P101" s="61">
+        <v>-1</v>
+      </c>
+      <c r="Q101" s="66">
+        <v>5</v>
+      </c>
+      <c r="R101" s="61">
+        <v>1</v>
+      </c>
+      <c r="S101" s="62">
+        <v>4</v>
+      </c>
+      <c r="T101" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O102" s="1">
+        <v>98</v>
+      </c>
+      <c r="P102" s="61">
+        <v>-2</v>
+      </c>
+      <c r="Q102" s="66">
+        <v>5</v>
+      </c>
+      <c r="R102" s="61">
+        <v>1</v>
+      </c>
+      <c r="S102" s="62">
+        <v>3</v>
+      </c>
+      <c r="T102" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="15:20" x14ac:dyDescent="0.25">
+      <c r="O103" s="1">
+        <v>99</v>
+      </c>
+      <c r="P103" s="61">
+        <v>-3</v>
+      </c>
+      <c r="Q103" s="66">
+        <v>5</v>
+      </c>
+      <c r="R103" s="61">
+        <v>1</v>
+      </c>
+      <c r="S103" s="62">
+        <v>2</v>
+      </c>
+      <c r="T103" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="15:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O104" s="1">
+        <v>100</v>
+      </c>
+      <c r="P104" s="63">
+        <v>-4</v>
+      </c>
+      <c r="Q104" s="67">
+        <v>5</v>
+      </c>
+      <c r="R104" s="63">
+        <v>1</v>
+      </c>
+      <c r="S104" s="64">
+        <v>1</v>
+      </c>
+      <c r="T104" s="23">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>